<commit_message>
Update Cheetah automation testing cases
</commit_message>
<xml_diff>
--- a/testcase/Cheetah-TestCase.xlsx
+++ b/testcase/Cheetah-TestCase.xlsx
@@ -10,7 +10,7 @@
     <sheet name="cheetah" sheetId="9" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cheetah!$C$1:$C$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cheetah!$M$1:$M$90</definedName>
     <definedName name="百度搜索页面">#REF!</definedName>
     <definedName name="关键字">#REF!</definedName>
     <definedName name="通用">#REF!</definedName>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111">
   <si>
     <t>用例编号</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>ParentNode=系统配置,ChildNode=仿真点管理</t>
+  </si>
+  <si>
+    <t>IP名称#18</t>
+  </si>
+  <si>
+    <t>text=Automation testing,text1=&lt;Keys.TAB&gt;,text2=127.0.0.2</t>
   </si>
 </sst>
 </file>
@@ -358,10 +364,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -397,25 +403,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,83 +424,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -524,16 +452,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,6 +483,75 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -586,175 +592,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,68 +789,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,151 +825,210 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1413,9 +1419,9 @@
   <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.625" defaultRowHeight="16.8"/>
@@ -2527,26 +2533,44 @@
       <c r="G45" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" ht="17.6" spans="1:8">
+      <c r="H45" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" ht="18" spans="1:8">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" ht="17.6" spans="1:8">
+      <c r="D46" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" ht="18" spans="1:8">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="D47" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="G47" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="H47" s="4"/>
     </row>
     <row r="48" ht="17.6" spans="1:8">
@@ -2980,9 +3004,8 @@
       <c r="H90" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C90"/>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="E1 E46:E1048576" errorStyle="information"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="E1 E48:E1048576" errorStyle="information"/>
     <dataValidation allowBlank="1" showInputMessage="1" sqref="G12 G17 G27 G43"/>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>